<commit_message>
importantly, divided daylight alpha opic by luminous flux for equivalent daylight in spdtoalpha opics
</commit_message>
<xml_diff>
--- a/Standards/CIES026_E2018/CIE_S026_Alpha_Opic_Toolbox_V1_049a_2020_Nov.xlsx
+++ b/Standards/CIES026_E2018/CIE_S026_Alpha_Opic_Toolbox_V1_049a_2020_Nov.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Box\Lighting Research Group\WilliamCoulter\Gantt Chart Deliverables\Software\Matlab_PNNL_Paper_Project\Project\Project_Data\Standards\CIES026_E2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/087cdde7941d7cda/MyMatlab/MetaMetric/Standards/CIES026_E2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE8CCC2-F103-4779-8497-E31CB2E30FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{BCE8CCC2-F103-4779-8497-E31CB2E30FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9EA5365-79C6-492C-A731-C5BE9541BB76}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1379,7 +1379,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>